<commit_message>
framework developed. Reports and read from excel added. End2End test case created and added. AjaxFactory for waiters added
</commit_message>
<xml_diff>
--- a/src/test/resources/input_data.xlsx
+++ b/src/test/resources/input_data.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
   <si>
     <t>TCID</t>
   </si>
@@ -28,6 +28,15 @@
     <t>Gender</t>
   </si>
   <si>
+    <t>ProductName</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>SearchCountry</t>
+  </si>
+  <si>
     <t>TC01</t>
   </si>
   <si>
@@ -41,13 +50,37 @@
   </si>
   <si>
     <t>TC02</t>
+  </si>
+  <si>
+    <t>TC03</t>
+  </si>
+  <si>
+    <t>Pabla</t>
+  </si>
+  <si>
+    <t>p.perez@gmail.com</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>Nokia Edge</t>
+  </si>
+  <si>
+    <t>United States of America</t>
+  </si>
+  <si>
+    <t>uni</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -61,12 +94,18 @@
       <name val="Calibri"/>
     </font>
     <font>
+      <b/>
+      <sz val="12.0"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -79,12 +118,6 @@
         <bgColor rgb="FFB7B7B7"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border/>
@@ -92,17 +125,18 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -337,38 +371,89 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="3"/>
+      <c r="S1" s="3"/>
+      <c r="T1" s="3"/>
+      <c r="U1" s="3"/>
+      <c r="V1" s="3"/>
+      <c r="W1" s="3"/>
+      <c r="X1" s="3"/>
+      <c r="Y1" s="3"/>
+      <c r="Z1" s="3"/>
     </row>
     <row r="2">
-      <c r="A2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="3">
+      <c r="A2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="4">
         <v>1234.0</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>8</v>
+      <c r="E2" s="4" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>8</v>
+      <c r="C3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
data driven locators added for the HomePage object. AbstractLocatorsPage created to make possible the ddLocators. Excels for DD also added.
</commit_message>
<xml_diff>
--- a/src/test/resources/input_data.xlsx
+++ b/src/test/resources/input_data.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
   <si>
     <t>TCID</t>
   </si>
@@ -74,6 +74,18 @@
   </si>
   <si>
     <t>uni</t>
+  </si>
+  <si>
+    <t>TC04</t>
+  </si>
+  <si>
+    <t>Blackberry</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>ind</t>
   </si>
 </sst>
 </file>
@@ -456,6 +468,20 @@
         <v>20</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>